<commit_message>
Add support for MacOS
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\automated_whatsapp-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vikrantarya/Desktop/automated_whatsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1684775A-A277-4EF6-8679-D100A97541AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB633B2-07EB-3B46-9AA6-8CB2495A4F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -52,12 +52,10 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Vishw Bhosdike</t>
-  </si>
-  <si>
-    <t>Formal yo_x000D_
-_x000D_
-Regards</t>
+    <t>Vikrant</t>
+  </si>
+  <si>
+    <t>how are you?</t>
   </si>
   <si>
     <t>This is informal message.</t>
@@ -72,13 +70,10 @@
     <t>Y</t>
   </si>
   <si>
-    <t>9825018513</t>
-  </si>
-  <si>
-    <t>+919825018513</t>
-  </si>
-  <si>
-    <t>919825018513</t>
+    <t>919289907889</t>
+  </si>
+  <si>
+    <t>+919289907889</t>
   </si>
   <si>
     <t>982501851</t>
@@ -118,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,12 +456,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,12 +490,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>9825018513</v>
+        <v>9289907889</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -521,42 +516,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3">
+        <v>9289907889</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
@@ -565,7 +560,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I1 A6:I6 A4:G5 A3:H3 A2:G2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:I1 A3:H3 A2:G2 A6:H6 A4:G4 A5:G5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>